<commit_message>
importar con el excel
deberia funcionar pero esta en pañales, y hay una cosa rara con la forma de tomar el tipo de activo, no lo toma nose porke
</commit_message>
<xml_diff>
--- a/sqat/public/excel/ImportarDatos.xlsx
+++ b/sqat/public/excel/ImportarDatos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigoalonsodomingu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigoalonsodomingu\Desktop\proyectos\Sistema-Gestor-de-Activos\sqat\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22AF7E85-6F2A-48CB-8A70-6EE71F31AD48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3172C2B5-2966-4A6C-9BF3-E418B7EC71E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{63237FC5-12C3-49CE-B41B-20BFD7A0CF2B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>rut</t>
   </si>
@@ -78,6 +78,33 @@
   </si>
   <si>
     <t>ubicación</t>
+  </si>
+  <si>
+    <t>nro_serie</t>
+  </si>
+  <si>
+    <t>marca</t>
+  </si>
+  <si>
+    <t>modelo</t>
+  </si>
+  <si>
+    <t>tipo de activo</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>usuario de activo</t>
+  </si>
+  <si>
+    <t>responsable de activo</t>
+  </si>
+  <si>
+    <t>precio</t>
+  </si>
+  <si>
+    <t>justificacion doble activo</t>
   </si>
 </sst>
 </file>
@@ -449,21 +476,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2165555-444A-4B0F-8252-37707CE7818F}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="25.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -505,6 +526,33 @@
       </c>
       <c r="N1" t="s">
         <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>